<commit_message>
Sua lai doan xem diem
</commit_message>
<xml_diff>
--- a/form_collectdata/form_collect/DataBase/db.xlsx
+++ b/form_collectdata/form_collect/DataBase/db.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Works\Tmp\Std-D20-DATN\Thutuc-BV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - ptit.edu.vn\Documents\Học\FormstoExcel\form_collectdata\form_collect\DataBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7056"/>
   </bookViews>
   <sheets>
     <sheet name="DS Hội đồng_DN" sheetId="1" r:id="rId1"/>
@@ -3633,6 +3633,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3666,19 +3676,6 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3691,14 +3688,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4044,33 +4044,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.69921875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" customWidth="1"/>
-    <col min="2" max="2" width="29.75" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" customWidth="1"/>
+    <col min="1" max="1" width="7.69921875" customWidth="1"/>
+    <col min="2" max="2" width="29.69921875" customWidth="1"/>
+    <col min="3" max="3" width="9.69921875" customWidth="1"/>
     <col min="4" max="4" width="10.5" customWidth="1"/>
-    <col min="5" max="11" width="7.6640625" customWidth="1"/>
+    <col min="5" max="11" width="7.69921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="51.75" customHeight="1">
-      <c r="A1" s="214" t="s">
+      <c r="A1" s="220" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="213"/>
-      <c r="C1" s="213"/>
-      <c r="D1" s="213"/>
+      <c r="B1" s="219"/>
+      <c r="C1" s="219"/>
+      <c r="D1" s="219"/>
     </row>
     <row r="2" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A2" s="212" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="213"/>
-      <c r="C2" s="213"/>
+      <c r="A2" s="218" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="219"/>
+      <c r="C2" s="219"/>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:6" ht="14.25" customHeight="1">
@@ -4193,11 +4193,11 @@
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A11" s="212" t="s">
+      <c r="A11" s="218" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="213"/>
-      <c r="C11" s="213"/>
+      <c r="B11" s="219"/>
+      <c r="C11" s="219"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:6" ht="14.25" customHeight="1">
@@ -4317,11 +4317,11 @@
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A20" s="212" t="s">
+      <c r="A20" s="218" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="213"/>
-      <c r="C20" s="213"/>
+      <c r="B20" s="219"/>
+      <c r="C20" s="219"/>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:6" ht="14.25" customHeight="1">
@@ -4441,11 +4441,11 @@
       <c r="D28" s="1"/>
     </row>
     <row r="29" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A29" s="212" t="s">
+      <c r="A29" s="218" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="213"/>
-      <c r="C29" s="213"/>
+      <c r="B29" s="219"/>
+      <c r="C29" s="219"/>
       <c r="D29" s="1"/>
     </row>
     <row r="30" spans="1:6" ht="14.25" customHeight="1">
@@ -4565,11 +4565,11 @@
       <c r="D37" s="1"/>
     </row>
     <row r="38" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A38" s="212" t="s">
+      <c r="A38" s="218" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="213"/>
-      <c r="C38" s="213"/>
+      <c r="B38" s="219"/>
+      <c r="C38" s="219"/>
       <c r="D38" s="1"/>
     </row>
     <row r="39" spans="1:6" ht="14.25" customHeight="1">
@@ -4689,11 +4689,11 @@
       <c r="D46" s="1"/>
     </row>
     <row r="47" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A47" s="212" t="s">
+      <c r="A47" s="218" t="s">
         <v>50</v>
       </c>
-      <c r="B47" s="213"/>
-      <c r="C47" s="213"/>
+      <c r="B47" s="219"/>
+      <c r="C47" s="219"/>
       <c r="D47" s="1"/>
     </row>
     <row r="48" spans="1:6" ht="14.25" customHeight="1">
@@ -4880,7 +4880,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="17.5" customHeight="1">
+    <row r="61" spans="1:6" ht="17.55" customHeight="1">
       <c r="A61" s="4">
         <v>4</v>
       </c>
@@ -5054,20 +5054,20 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.69921875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11.25" customWidth="1"/>
-    <col min="3" max="3" width="11.4140625" customWidth="1"/>
-    <col min="4" max="4" width="6.4140625" customWidth="1"/>
-    <col min="5" max="5" width="8.9140625" customWidth="1"/>
+    <col min="1" max="1" width="2.69921875" customWidth="1"/>
+    <col min="2" max="2" width="11.19921875" customWidth="1"/>
+    <col min="3" max="3" width="11.3984375" customWidth="1"/>
+    <col min="4" max="4" width="6.3984375" customWidth="1"/>
+    <col min="5" max="5" width="8.8984375" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="7" max="7" width="12.9140625" customWidth="1"/>
-    <col min="8" max="8" width="7.1640625" customWidth="1"/>
-    <col min="9" max="9" width="6.4140625" customWidth="1"/>
-    <col min="10" max="10" width="38.9140625" customWidth="1"/>
-    <col min="11" max="11" width="7.9140625" customWidth="1"/>
-    <col min="12" max="12" width="6.25" customWidth="1"/>
+    <col min="7" max="7" width="12.8984375" customWidth="1"/>
+    <col min="8" max="8" width="7.19921875" customWidth="1"/>
+    <col min="9" max="9" width="6.3984375" customWidth="1"/>
+    <col min="10" max="10" width="38.8984375" customWidth="1"/>
+    <col min="11" max="11" width="7.8984375" customWidth="1"/>
+    <col min="12" max="12" width="6.19921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="14.25" customHeight="1">
@@ -5123,10 +5123,10 @@
       <c r="B4" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="215" t="s">
+      <c r="C4" s="221" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="216"/>
+      <c r="D4" s="222"/>
       <c r="E4" s="30" t="s">
         <v>65</v>
       </c>
@@ -5793,10 +5793,10 @@
       <c r="B24" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="215" t="s">
+      <c r="C24" s="221" t="s">
         <v>3</v>
       </c>
-      <c r="D24" s="216"/>
+      <c r="D24" s="222"/>
       <c r="E24" s="30" t="s">
         <v>65</v>
       </c>
@@ -6441,10 +6441,10 @@
       <c r="B44" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="C44" s="215" t="s">
+      <c r="C44" s="221" t="s">
         <v>3</v>
       </c>
-      <c r="D44" s="216"/>
+      <c r="D44" s="222"/>
       <c r="E44" s="30" t="s">
         <v>65</v>
       </c>
@@ -7129,10 +7129,10 @@
       <c r="B65" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="C65" s="215" t="s">
+      <c r="C65" s="221" t="s">
         <v>3</v>
       </c>
-      <c r="D65" s="216"/>
+      <c r="D65" s="222"/>
       <c r="E65" s="30" t="s">
         <v>65</v>
       </c>
@@ -7783,10 +7783,10 @@
       <c r="B84" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="C84" s="215" t="s">
+      <c r="C84" s="221" t="s">
         <v>3</v>
       </c>
-      <c r="D84" s="216"/>
+      <c r="D84" s="222"/>
       <c r="E84" s="30" t="s">
         <v>65</v>
       </c>
@@ -8421,10 +8421,10 @@
       <c r="B103" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="C103" s="215" t="s">
+      <c r="C103" s="221" t="s">
         <v>3</v>
       </c>
-      <c r="D103" s="216"/>
+      <c r="D103" s="222"/>
       <c r="E103" s="30" t="s">
         <v>65</v>
       </c>
@@ -9023,10 +9023,10 @@
       <c r="B121" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="C121" s="215" t="s">
+      <c r="C121" s="221" t="s">
         <v>3</v>
       </c>
-      <c r="D121" s="216"/>
+      <c r="D121" s="222"/>
       <c r="E121" s="30" t="s">
         <v>65</v>
       </c>
@@ -9674,25 +9674,25 @@
   </sheetPr>
   <dimension ref="A1:M137"/>
   <sheetViews>
-    <sheetView topLeftCell="A118" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A133" sqref="A133:XFD133"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.69921875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="5.9140625" customWidth="1"/>
-    <col min="2" max="2" width="11.25" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="6.4140625" customWidth="1"/>
-    <col min="5" max="5" width="8.9140625" customWidth="1"/>
-    <col min="6" max="6" width="9.9140625" customWidth="1"/>
-    <col min="7" max="7" width="19.1640625" customWidth="1"/>
-    <col min="8" max="8" width="9.9140625" customWidth="1"/>
-    <col min="9" max="9" width="7.6640625" customWidth="1"/>
-    <col min="10" max="10" width="91.25" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" customWidth="1"/>
-    <col min="12" max="12" width="7.75" customWidth="1"/>
-    <col min="13" max="13" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="5.8984375" customWidth="1"/>
+    <col min="2" max="2" width="11.19921875" customWidth="1"/>
+    <col min="3" max="3" width="10.69921875" customWidth="1"/>
+    <col min="4" max="4" width="6.3984375" customWidth="1"/>
+    <col min="5" max="5" width="8.8984375" customWidth="1"/>
+    <col min="6" max="6" width="9.8984375" customWidth="1"/>
+    <col min="7" max="7" width="19.19921875" customWidth="1"/>
+    <col min="8" max="8" width="9.8984375" customWidth="1"/>
+    <col min="9" max="9" width="7.69921875" customWidth="1"/>
+    <col min="10" max="10" width="91.19921875" customWidth="1"/>
+    <col min="11" max="11" width="12.69921875" customWidth="1"/>
+    <col min="12" max="12" width="7.69921875" customWidth="1"/>
+    <col min="13" max="13" width="14.69921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.25" customHeight="1">
@@ -9743,10 +9743,10 @@
       <c r="B4" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="219" t="s">
+      <c r="C4" s="225" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="218"/>
+      <c r="D4" s="224"/>
       <c r="E4" s="67" t="s">
         <v>65</v>
       </c>
@@ -10445,10 +10445,10 @@
       <c r="B24" s="87" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="220" t="s">
+      <c r="C24" s="226" t="s">
         <v>3</v>
       </c>
-      <c r="D24" s="218"/>
+      <c r="D24" s="224"/>
       <c r="E24" s="87" t="s">
         <v>65</v>
       </c>
@@ -10992,7 +10992,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="16" customHeight="1">
+    <row r="38" spans="1:13" ht="16.05" customHeight="1">
       <c r="A38" s="89">
         <v>14</v>
       </c>
@@ -11123,10 +11123,10 @@
       <c r="B44" s="104" t="s">
         <v>64</v>
       </c>
-      <c r="C44" s="221" t="s">
+      <c r="C44" s="227" t="s">
         <v>3</v>
       </c>
-      <c r="D44" s="218"/>
+      <c r="D44" s="224"/>
       <c r="E44" s="104" t="s">
         <v>65</v>
       </c>
@@ -11841,10 +11841,10 @@
       <c r="B65" s="122" t="s">
         <v>64</v>
       </c>
-      <c r="C65" s="222" t="s">
+      <c r="C65" s="228" t="s">
         <v>3</v>
       </c>
-      <c r="D65" s="218"/>
+      <c r="D65" s="224"/>
       <c r="E65" s="122" t="s">
         <v>65</v>
       </c>
@@ -12535,10 +12535,10 @@
       <c r="B84" s="137" t="s">
         <v>64</v>
       </c>
-      <c r="C84" s="223" t="s">
+      <c r="C84" s="229" t="s">
         <v>3</v>
       </c>
-      <c r="D84" s="218"/>
+      <c r="D84" s="224"/>
       <c r="E84" s="137" t="s">
         <v>65</v>
       </c>
@@ -13202,10 +13202,10 @@
       <c r="B103" s="151" t="s">
         <v>64</v>
       </c>
-      <c r="C103" s="224" t="s">
+      <c r="C103" s="230" t="s">
         <v>3</v>
       </c>
-      <c r="D103" s="218"/>
+      <c r="D103" s="224"/>
       <c r="E103" s="151" t="s">
         <v>65</v>
       </c>
@@ -13830,10 +13830,10 @@
       <c r="B121" s="167" t="s">
         <v>64</v>
       </c>
-      <c r="C121" s="217" t="s">
+      <c r="C121" s="223" t="s">
         <v>3</v>
       </c>
-      <c r="D121" s="218"/>
+      <c r="D121" s="224"/>
       <c r="E121" s="167" t="s">
         <v>65</v>
       </c>
@@ -14496,12 +14496,12 @@
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.69921875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="19.9140625" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" customWidth="1"/>
-    <col min="3" max="3" width="22.25" customWidth="1"/>
-    <col min="4" max="11" width="7.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.8984375" customWidth="1"/>
+    <col min="2" max="2" width="7.69921875" customWidth="1"/>
+    <col min="3" max="3" width="22.19921875" customWidth="1"/>
+    <col min="4" max="11" width="7.69921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="14.25" customHeight="1">
@@ -14973,56 +14973,56 @@
   </sheetPr>
   <dimension ref="A1:M202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I186" workbookViewId="0">
+    <sheetView topLeftCell="A69" workbookViewId="0">
       <selection activeCell="M200" sqref="M200"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.69921875" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="3.5" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.4140625" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" customWidth="1"/>
-    <col min="5" max="5" width="8.9140625" customWidth="1"/>
-    <col min="6" max="6" width="7.6640625" customWidth="1"/>
-    <col min="7" max="7" width="22.25" customWidth="1"/>
-    <col min="8" max="9" width="7.6640625" customWidth="1"/>
-    <col min="10" max="10" width="98.6640625" customWidth="1"/>
-    <col min="11" max="11" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="7.69921875" customWidth="1"/>
+    <col min="3" max="3" width="13.3984375" customWidth="1"/>
+    <col min="4" max="4" width="7.69921875" customWidth="1"/>
+    <col min="5" max="5" width="8.8984375" customWidth="1"/>
+    <col min="6" max="6" width="7.69921875" customWidth="1"/>
+    <col min="7" max="7" width="22.19921875" customWidth="1"/>
+    <col min="8" max="9" width="7.69921875" customWidth="1"/>
+    <col min="10" max="10" width="98.69921875" customWidth="1"/>
+    <col min="11" max="11" width="7.69921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.25" customHeight="1"/>
     <row r="2" spans="1:13" ht="14.25" customHeight="1">
-      <c r="A2" s="232" t="s">
+      <c r="A2" s="231" t="s">
         <v>561</v>
       </c>
-      <c r="B2" s="213"/>
-      <c r="C2" s="213"/>
-      <c r="D2" s="213"/>
-      <c r="E2" s="213"/>
-      <c r="F2" s="213"/>
+      <c r="B2" s="219"/>
+      <c r="C2" s="219"/>
+      <c r="D2" s="219"/>
+      <c r="E2" s="219"/>
+      <c r="F2" s="219"/>
       <c r="G2" s="185"/>
-      <c r="H2" s="232" t="s">
+      <c r="H2" s="231" t="s">
         <v>562</v>
       </c>
-      <c r="I2" s="213"/>
-      <c r="J2" s="213"/>
+      <c r="I2" s="219"/>
+      <c r="J2" s="219"/>
     </row>
     <row r="3" spans="1:13" ht="14.25" customHeight="1">
-      <c r="A3" s="233" t="s">
+      <c r="A3" s="232" t="s">
         <v>563</v>
       </c>
-      <c r="B3" s="213"/>
-      <c r="C3" s="213"/>
-      <c r="D3" s="213"/>
-      <c r="E3" s="213"/>
-      <c r="F3" s="213"/>
+      <c r="B3" s="219"/>
+      <c r="C3" s="219"/>
+      <c r="D3" s="219"/>
+      <c r="E3" s="219"/>
+      <c r="F3" s="219"/>
       <c r="G3" s="185"/>
-      <c r="H3" s="233" t="s">
+      <c r="H3" s="232" t="s">
         <v>564</v>
       </c>
-      <c r="I3" s="213"/>
-      <c r="J3" s="213"/>
+      <c r="I3" s="219"/>
+      <c r="J3" s="219"/>
     </row>
     <row r="4" spans="1:13" ht="14.25" customHeight="1">
       <c r="A4" s="186"/>
@@ -15044,11 +15044,11 @@
       <c r="E5" s="187"/>
       <c r="F5" s="186"/>
       <c r="G5" s="185"/>
-      <c r="H5" s="234" t="s">
+      <c r="H5" s="233" t="s">
         <v>565</v>
       </c>
-      <c r="I5" s="213"/>
-      <c r="J5" s="213"/>
+      <c r="I5" s="219"/>
+      <c r="J5" s="219"/>
     </row>
     <row r="6" spans="1:13" ht="14.25" customHeight="1">
       <c r="A6" s="186"/>
@@ -15063,32 +15063,32 @@
       <c r="J6" s="185"/>
     </row>
     <row r="7" spans="1:13" ht="14.25" customHeight="1">
-      <c r="A7" s="235" t="s">
+      <c r="A7" s="234" t="s">
         <v>566</v>
       </c>
-      <c r="B7" s="213"/>
-      <c r="C7" s="213"/>
-      <c r="D7" s="213"/>
-      <c r="E7" s="213"/>
-      <c r="F7" s="213"/>
-      <c r="G7" s="213"/>
-      <c r="H7" s="213"/>
-      <c r="I7" s="213"/>
-      <c r="J7" s="213"/>
+      <c r="B7" s="219"/>
+      <c r="C7" s="219"/>
+      <c r="D7" s="219"/>
+      <c r="E7" s="219"/>
+      <c r="F7" s="219"/>
+      <c r="G7" s="219"/>
+      <c r="H7" s="219"/>
+      <c r="I7" s="219"/>
+      <c r="J7" s="219"/>
     </row>
     <row r="8" spans="1:13" ht="14.25" customHeight="1">
-      <c r="A8" s="235" t="s">
+      <c r="A8" s="234" t="s">
         <v>567</v>
       </c>
-      <c r="B8" s="213"/>
-      <c r="C8" s="213"/>
-      <c r="D8" s="213"/>
-      <c r="E8" s="213"/>
-      <c r="F8" s="213"/>
-      <c r="G8" s="213"/>
-      <c r="H8" s="213"/>
-      <c r="I8" s="213"/>
-      <c r="J8" s="213"/>
+      <c r="B8" s="219"/>
+      <c r="C8" s="219"/>
+      <c r="D8" s="219"/>
+      <c r="E8" s="219"/>
+      <c r="F8" s="219"/>
+      <c r="G8" s="219"/>
+      <c r="H8" s="219"/>
+      <c r="I8" s="219"/>
+      <c r="J8" s="219"/>
     </row>
     <row r="9" spans="1:13" ht="14.25" customHeight="1">
       <c r="A9" s="186"/>
@@ -15104,35 +15104,35 @@
     </row>
     <row r="10" spans="1:13" ht="14.25" customHeight="1">
       <c r="A10" s="186"/>
-      <c r="B10" s="225" t="s">
+      <c r="B10" s="235" t="s">
         <v>568</v>
       </c>
-      <c r="C10" s="213"/>
+      <c r="C10" s="219"/>
       <c r="D10" s="186"/>
       <c r="E10" s="187"/>
       <c r="F10" s="186"/>
-      <c r="G10" s="226" t="s">
+      <c r="G10" s="236" t="s">
         <v>569</v>
       </c>
-      <c r="H10" s="213"/>
+      <c r="H10" s="219"/>
       <c r="I10" s="186"/>
       <c r="J10" s="185"/>
     </row>
     <row r="11" spans="1:13" ht="14.25" customHeight="1">
       <c r="A11" s="186"/>
-      <c r="B11" s="227" t="s">
+      <c r="B11" s="237" t="s">
         <v>570</v>
       </c>
-      <c r="C11" s="228"/>
-      <c r="D11" s="229"/>
+      <c r="C11" s="238"/>
+      <c r="D11" s="239"/>
       <c r="E11" s="187"/>
       <c r="F11" s="186"/>
-      <c r="G11" s="230" t="s">
+      <c r="G11" s="240" t="s">
         <v>571</v>
       </c>
-      <c r="H11" s="228"/>
-      <c r="I11" s="228"/>
-      <c r="J11" s="229"/>
+      <c r="H11" s="238"/>
+      <c r="I11" s="238"/>
+      <c r="J11" s="239"/>
     </row>
     <row r="12" spans="1:13" ht="14.25" customHeight="1">
       <c r="A12" s="188"/>
@@ -15153,10 +15153,10 @@
       <c r="B13" s="192" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="231" t="s">
+      <c r="C13" s="241" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="218"/>
+      <c r="D13" s="224"/>
       <c r="E13" s="192" t="s">
         <v>65</v>
       </c>
@@ -15178,7 +15178,7 @@
       <c r="K13" s="193" t="s">
         <v>573</v>
       </c>
-      <c r="M13" s="241" t="s">
+      <c r="M13" s="217" t="s">
         <v>813</v>
       </c>
     </row>
@@ -22328,6 +22328,11 @@
   </sheetData>
   <autoFilter ref="A13:K202"/>
   <mergeCells count="12">
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="G11:J11"/>
+    <mergeCell ref="C13:D13"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="H3:J3"/>
@@ -22335,11 +22340,6 @@
     <mergeCell ref="A8:J8"/>
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="A7:J7"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="G11:J11"/>
-    <mergeCell ref="C13:D13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup scale="58" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -22354,31 +22354,31 @@
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="6.58203125" customWidth="1"/>
-    <col min="3" max="3" width="22.25" style="240" customWidth="1"/>
-    <col min="4" max="4" width="25.33203125" style="240" customWidth="1"/>
-    <col min="5" max="5" width="26.25" customWidth="1"/>
-    <col min="6" max="6" width="26.25" style="240" customWidth="1"/>
-    <col min="7" max="10" width="26.25" style="210" customWidth="1"/>
-    <col min="11" max="11" width="14.1640625" customWidth="1"/>
+    <col min="1" max="1" width="14.69921875" customWidth="1"/>
+    <col min="2" max="2" width="6.59765625" customWidth="1"/>
+    <col min="3" max="3" width="22.19921875" style="216" customWidth="1"/>
+    <col min="4" max="4" width="25.296875" style="216" customWidth="1"/>
+    <col min="5" max="5" width="26.19921875" customWidth="1"/>
+    <col min="6" max="6" width="26.19921875" style="216" customWidth="1"/>
+    <col min="7" max="10" width="26.19921875" style="210" customWidth="1"/>
+    <col min="11" max="11" width="14.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="70">
-      <c r="A1" s="236" t="s">
+    <row r="1" spans="1:14" ht="69">
+      <c r="A1" s="212" t="s">
         <v>71</v>
       </c>
       <c r="B1">
         <f>VLOOKUP(A1,$K$1:$L$189,2,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="C1" s="240" t="str">
+      <c r="C1" s="216" t="str">
         <f>VLOOKUP(A1,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Nghiên cứu, thiết kế thiết bị thu âm tiếng nói và truyền không dây qua sóng RF sử dụng kit STM và microphone MEMS</v>
       </c>
-      <c r="D1" s="240" t="str">
+      <c r="D1" s="216" t="str">
         <f>VLOOKUP(A1,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Nghiên cứu, thiết kế thiết bị thu âm tiếng nói và truyền không dây qua sóng RF sử dụng kit STM và microphone MEMS</v>
       </c>
@@ -22386,7 +22386,7 @@
         <f>IF(TRIM(UPPER(C1))&lt;&gt;TRIM(UPPER(D1)),"Error","")</f>
         <v/>
       </c>
-      <c r="F1" s="240" t="s">
+      <c r="F1" s="216" t="s">
         <v>814</v>
       </c>
       <c r="G1" s="210" t="str">
@@ -22416,19 +22416,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="28">
-      <c r="A2" s="236" t="s">
+    <row r="2" spans="1:14" ht="27.6">
+      <c r="A2" s="212" t="s">
         <v>80</v>
       </c>
       <c r="B2" s="210">
         <f t="shared" ref="B2:B65" si="0">VLOOKUP(A2,$K$1:$L$189,2,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="C2" s="240" t="str">
+      <c r="C2" s="216" t="str">
         <f>VLOOKUP(A2,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Hệ thống cảnh báo tài xế ngủ gật trên oto</v>
       </c>
-      <c r="D2" s="240" t="str">
+      <c r="D2" s="216" t="str">
         <f>VLOOKUP(A2,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Hệ thống cảnh báo tài xế ngủ gật trên oto</v>
       </c>
@@ -22463,19 +22463,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="42">
-      <c r="A3" s="236" t="s">
+    <row r="3" spans="1:14" ht="41.4">
+      <c r="A3" s="212" t="s">
         <v>85</v>
       </c>
       <c r="B3" s="210">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C3" s="240" t="str">
+      <c r="C3" s="216" t="str">
         <f>VLOOKUP(A3,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Hệ thống hỗ trợ vận hành Wireless Audio Visual System vừa và nhỏ.</v>
       </c>
-      <c r="D3" s="240" t="str">
+      <c r="D3" s="216" t="str">
         <f>VLOOKUP(A3,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Hệ thống hỗ trợ vận hành Wireless Audio Visual System vừa và nhỏ.</v>
       </c>
@@ -22510,19 +22510,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="28">
-      <c r="A4" s="236" t="s">
+    <row r="4" spans="1:14" ht="27.6">
+      <c r="A4" s="212" t="s">
         <v>90</v>
       </c>
       <c r="B4" s="210">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C4" s="240" t="str">
+      <c r="C4" s="216" t="str">
         <f>VLOOKUP(A4,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v xml:space="preserve"> Xây dựng bãi đỗ xe tự động </v>
       </c>
-      <c r="D4" s="240" t="str">
+      <c r="D4" s="216" t="str">
         <f>VLOOKUP(A4,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v xml:space="preserve"> Xây dựng bãi đỗ xe tự động </v>
       </c>
@@ -22557,19 +22557,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="56">
-      <c r="A5" s="236" t="s">
+    <row r="5" spans="1:14" ht="55.2">
+      <c r="A5" s="212" t="s">
         <v>96</v>
       </c>
       <c r="B5" s="210">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C5" s="240" t="str">
+      <c r="C5" s="216" t="str">
         <f>VLOOKUP(A5,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Thiết kế và tối ưu hóa PCB chống nhiễu điện từ (EMI) mạch ESP32 và SIM800C</v>
       </c>
-      <c r="D5" s="240" t="str">
+      <c r="D5" s="216" t="str">
         <f>VLOOKUP(A5,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Thiết kế và tối ưu hóa PCB chống nhiễu điện từ (EMI) mạch ESP32 và SIM800C</v>
       </c>
@@ -22604,19 +22604,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="42">
-      <c r="A6" s="236" t="s">
+    <row r="6" spans="1:14" ht="41.4">
+      <c r="A6" s="212" t="s">
         <v>102</v>
       </c>
       <c r="B6" s="210">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C6" s="240" t="str">
+      <c r="C6" s="216" t="str">
         <f>VLOOKUP(A6,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Nghiên cứu tổng quan về BLE hướng tới phát triển ứng dụng Web BLE</v>
       </c>
-      <c r="D6" s="240" t="str">
+      <c r="D6" s="216" t="str">
         <f>VLOOKUP(A6,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Nghiên cứu tổng quan về BLE hướng tới phát triển ứng dụng Web BLE</v>
       </c>
@@ -22651,19 +22651,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="42">
-      <c r="A7" s="236" t="s">
+    <row r="7" spans="1:14" ht="41.4">
+      <c r="A7" s="212" t="s">
         <v>107</v>
       </c>
       <c r="B7" s="210">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C7" s="240" t="str">
+      <c r="C7" s="216" t="str">
         <f>VLOOKUP(A7,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Thiết kế và xây dựng hệ thống nhà thông minh ứng dụng AI</v>
       </c>
-      <c r="D7" s="240" t="str">
+      <c r="D7" s="216" t="str">
         <f>VLOOKUP(A7,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Thiết kế và xây dựng hệ thống nhà thông minh ứng dụng AI</v>
       </c>
@@ -22698,19 +22698,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="42">
-      <c r="A8" s="236" t="s">
+    <row r="8" spans="1:14" ht="41.4">
+      <c r="A8" s="212" t="s">
         <v>113</v>
       </c>
       <c r="B8" s="210">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C8" s="240" t="str">
+      <c r="C8" s="216" t="str">
         <f>VLOOKUP(A8,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Thiết kế và chế tạo xe tự hành ứng dụng Slam tối ưu hóa đường đi</v>
       </c>
-      <c r="D8" s="240" t="str">
+      <c r="D8" s="216" t="str">
         <f>VLOOKUP(A8,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Thiết kế và chế tạo xe tự hành ứng dụng Slam tối ưu hóa đường đi</v>
       </c>
@@ -22746,18 +22746,18 @@
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="236" t="s">
+      <c r="A9" s="212" t="s">
         <v>120</v>
       </c>
       <c r="B9" s="210">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C9" s="240" t="str">
+      <c r="C9" s="216" t="str">
         <f>VLOOKUP(A9,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Xây dựng xe cân bằng</v>
       </c>
-      <c r="D9" s="240" t="str">
+      <c r="D9" s="216" t="str">
         <f>VLOOKUP(A9,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>xây dựng xe cân bằng</v>
       </c>
@@ -22792,19 +22792,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="56">
-      <c r="A10" s="236" t="s">
+    <row r="10" spans="1:14" ht="55.2">
+      <c r="A10" s="212" t="s">
         <v>124</v>
       </c>
       <c r="B10" s="210">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C10" s="240" t="str">
+      <c r="C10" s="216" t="str">
         <f>VLOOKUP(A10,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Xây dựng hệ thống giám sát và điều khiển vườn thông minh ứng dụng firebase</v>
       </c>
-      <c r="D10" s="240" t="str">
+      <c r="D10" s="216" t="str">
         <f>VLOOKUP(A10,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Xây dựng hệ thống giám sát và điều khiển vườn thông minh ứng dụng firebase</v>
       </c>
@@ -22839,19 +22839,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="56">
-      <c r="A11" s="236" t="s">
+    <row r="11" spans="1:14" ht="55.2">
+      <c r="A11" s="212" t="s">
         <v>130</v>
       </c>
       <c r="B11" s="210">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C11" s="240" t="str">
+      <c r="C11" s="216" t="str">
         <f>VLOOKUP(A11,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Xây dựng hệ thống quản lý nông nghiệp tự động ứng dụng công nghệ không dây</v>
       </c>
-      <c r="D11" s="240" t="str">
+      <c r="D11" s="216" t="str">
         <f>VLOOKUP(A11,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Xây dựng hệ thống quản lý nông nghiệp tự động ứng dụng công nghệ không dây</v>
       </c>
@@ -22886,19 +22886,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="42">
-      <c r="A12" s="236" t="s">
+    <row r="12" spans="1:14" ht="41.4">
+      <c r="A12" s="212" t="s">
         <v>135</v>
       </c>
       <c r="B12" s="210">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C12" s="240" t="str">
+      <c r="C12" s="216" t="str">
         <f>VLOOKUP(A12,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Xây dựng hệ thống giám sát và điều khiển toà nhà qua Web</v>
       </c>
-      <c r="D12" s="240" t="str">
+      <c r="D12" s="216" t="str">
         <f>VLOOKUP(A12,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Xây dựng hệ thống giám sát và điều khiển toà nhà qua Web</v>
       </c>
@@ -22933,19 +22933,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="28">
-      <c r="A13" s="236" t="s">
+    <row r="13" spans="1:14" ht="27.6">
+      <c r="A13" s="212" t="s">
         <v>140</v>
       </c>
       <c r="B13" s="210">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C13" s="240" t="str">
+      <c r="C13" s="216" t="str">
         <f>VLOOKUP(A13,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Hệ thống giám sát sức khỏe cá nhân</v>
       </c>
-      <c r="D13" s="240" t="str">
+      <c r="D13" s="216" t="str">
         <f>VLOOKUP(A13,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Hệ thống giám sát sức khỏe cá nhân</v>
       </c>
@@ -22980,19 +22980,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="56">
-      <c r="A14" s="236" t="s">
+    <row r="14" spans="1:14" ht="41.4">
+      <c r="A14" s="212" t="s">
         <v>145</v>
       </c>
       <c r="B14" s="210">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C14" s="240" t="str">
+      <c r="C14" s="216" t="str">
         <f>VLOOKUP(A14,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Xây dựng mô hình, thiết bị nhà thông minh ứng dụng công nghệ BLE mesh</v>
       </c>
-      <c r="D14" s="240" t="str">
+      <c r="D14" s="216" t="str">
         <f>VLOOKUP(A14,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Xây dựng mô hình, thiết bị nhà thông minh ứng dụng công nghệ BLE mesh</v>
       </c>
@@ -23027,19 +23027,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="28">
-      <c r="A15" s="236" t="s">
+    <row r="15" spans="1:14" ht="27.6">
+      <c r="A15" s="212" t="s">
         <v>149</v>
       </c>
       <c r="B15" s="210">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C15" s="240" t="str">
+      <c r="C15" s="216" t="str">
         <f>VLOOKUP(A15,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Cánh tay robot phân loại sản phẩm</v>
       </c>
-      <c r="D15" s="240" t="str">
+      <c r="D15" s="216" t="str">
         <f>VLOOKUP(A15,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Cánh tay robot phân loại sản phẩm</v>
       </c>
@@ -23074,19 +23074,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="28">
-      <c r="A16" s="236" t="s">
+    <row r="16" spans="1:14" ht="27.6">
+      <c r="A16" s="212" t="s">
         <v>154</v>
       </c>
       <c r="B16" s="210">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C16" s="240" t="str">
+      <c r="C16" s="216" t="str">
         <f>VLOOKUP(A16,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Xậy dựng hệ thống quản lý bãi đỗ xe</v>
       </c>
-      <c r="D16" s="240" t="str">
+      <c r="D16" s="216" t="str">
         <f>VLOOKUP(A16,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Xậy dựng hệ thống quản lý bãi đỗ xe</v>
       </c>
@@ -23121,7 +23121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="28">
+    <row r="17" spans="1:14" ht="27.6">
       <c r="A17" t="s">
         <v>159</v>
       </c>
@@ -23129,11 +23129,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C17" s="240" t="str">
+      <c r="C17" s="216" t="str">
         <f>VLOOKUP(A17,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Hệ thống nhận diện và theo dõi đối tượng</v>
       </c>
-      <c r="D17" s="240" t="str">
+      <c r="D17" s="216" t="str">
         <f>VLOOKUP(A17,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Hệ thống nhận diện và theo dõi đối tượng</v>
       </c>
@@ -23168,7 +23168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="56">
+    <row r="18" spans="1:14" ht="55.2">
       <c r="A18" t="s">
         <v>163</v>
       </c>
@@ -23176,11 +23176,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C18" s="240" t="str">
+      <c r="C18" s="216" t="str">
         <f>VLOOKUP(A18,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Nghiên cứu, xây dựng hệ thống phát hiện và cảnh báo cháy sử dụng Raspberry Pi.</v>
       </c>
-      <c r="D18" s="240" t="str">
+      <c r="D18" s="216" t="str">
         <f>VLOOKUP(A18,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Nghiên cứu, xây dựng hệ thống phát hiện và cảnh báo cháy sử dụng Raspberry Pi.</v>
       </c>
@@ -23215,7 +23215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="28">
+    <row r="19" spans="1:14" ht="27.6">
       <c r="A19" t="s">
         <v>168</v>
       </c>
@@ -23223,11 +23223,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C19" s="240" t="str">
+      <c r="C19" s="216" t="str">
         <f>VLOOKUP(A19,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Xây dựng hệ thống quản lý ra vào căn hộ</v>
       </c>
-      <c r="D19" s="240" t="str">
+      <c r="D19" s="216" t="str">
         <f>VLOOKUP(A19,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Xây dựng hệ thống quản lý ra vào căn hộ</v>
       </c>
@@ -23262,7 +23262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="28">
+    <row r="20" spans="1:14" ht="27.6">
       <c r="A20" t="s">
         <v>172</v>
       </c>
@@ -23270,11 +23270,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C20" s="240" t="str">
+      <c r="C20" s="216" t="str">
         <f>VLOOKUP(A20,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Xây dựng máy bay không người lái</v>
       </c>
-      <c r="D20" s="240" t="str">
+      <c r="D20" s="216" t="str">
         <f>VLOOKUP(A20,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Xây dựng máy bay không người lái</v>
       </c>
@@ -23309,7 +23309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="28">
+    <row r="21" spans="1:14" ht="27.6">
       <c r="A21" t="s">
         <v>177</v>
       </c>
@@ -23317,11 +23317,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C21" s="240" t="str">
+      <c r="C21" s="216" t="str">
         <f>VLOOKUP(A21,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Xây dựng bãi đỗ xe thông minh</v>
       </c>
-      <c r="D21" s="240" t="str">
+      <c r="D21" s="216" t="str">
         <f>VLOOKUP(A21,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Xây dựng bãi đỗ xe thông minh</v>
       </c>
@@ -23356,7 +23356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="42">
+    <row r="22" spans="1:14" ht="41.4">
       <c r="A22" t="s">
         <v>181</v>
       </c>
@@ -23364,11 +23364,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C22" s="240" t="str">
+      <c r="C22" s="216" t="str">
         <f>VLOOKUP(A22,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Xây dựng hệ thống điều khiển nhà thông minh bằng giọng nói</v>
       </c>
-      <c r="D22" s="240" t="str">
+      <c r="D22" s="216" t="str">
         <f>VLOOKUP(A22,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Xây dựng hệ thống điều khiển nhà thông minh bằng giọng nói</v>
       </c>
@@ -23376,7 +23376,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F22" s="240" t="s">
+      <c r="F22" s="216" t="s">
         <v>814</v>
       </c>
       <c r="G22" s="210" t="str">
@@ -23406,7 +23406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="42">
+    <row r="23" spans="1:14" ht="41.4">
       <c r="A23" t="s">
         <v>186</v>
       </c>
@@ -23414,11 +23414,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C23" s="240" t="str">
+      <c r="C23" s="216" t="str">
         <f>VLOOKUP(A23,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Nghiên cứu, chế tạo xe giao vận  hàng hóa trong kho hàng</v>
       </c>
-      <c r="D23" s="240" t="str">
+      <c r="D23" s="216" t="str">
         <f>VLOOKUP(A23,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Nghiên cứu, chế tạo xe giao vận  hàng hóa trong kho hàng</v>
       </c>
@@ -23426,7 +23426,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F23" s="240" t="s">
+      <c r="F23" s="216" t="s">
         <v>814</v>
       </c>
       <c r="G23" s="210" t="str">
@@ -23456,7 +23456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="28">
+    <row r="24" spans="1:14" ht="27.6">
       <c r="A24" t="s">
         <v>191</v>
       </c>
@@ -23464,11 +23464,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C24" s="240" t="str">
+      <c r="C24" s="216" t="str">
         <f>VLOOKUP(A24,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Giám sát nhịp tim qua điện thoại Android</v>
       </c>
-      <c r="D24" s="240" t="str">
+      <c r="D24" s="216" t="str">
         <f>VLOOKUP(A24,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Giám sát nhịp tim qua điện thoại Android</v>
       </c>
@@ -23476,7 +23476,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F24" s="240" t="s">
+      <c r="F24" s="216" t="s">
         <v>814</v>
       </c>
       <c r="G24" s="210" t="str">
@@ -23506,7 +23506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="42">
+    <row r="25" spans="1:14" ht="41.4">
       <c r="A25" t="s">
         <v>195</v>
       </c>
@@ -23514,11 +23514,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C25" s="240" t="str">
+      <c r="C25" s="216" t="str">
         <f>VLOOKUP(A25,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Hệ thống vườn thông minh sử dụng Raspberry Pi 3B</v>
       </c>
-      <c r="D25" s="240" t="str">
+      <c r="D25" s="216" t="str">
         <f>VLOOKUP(A25,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Hệ thống vườn thông minh sử dụng Raspberry Pi 3B</v>
       </c>
@@ -23553,7 +23553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="28">
+    <row r="26" spans="1:14" ht="27.6">
       <c r="A26" t="s">
         <v>199</v>
       </c>
@@ -23561,11 +23561,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C26" s="240" t="str">
+      <c r="C26" s="216" t="str">
         <f>VLOOKUP(A26,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Xây dựng nhà thông minh thông qua mạng Zigbee</v>
       </c>
-      <c r="D26" s="240" t="str">
+      <c r="D26" s="216" t="str">
         <f>VLOOKUP(A26,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Xây dựng nhà thông minh thông qua mạng Zigbee</v>
       </c>
@@ -23600,7 +23600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="56">
+    <row r="27" spans="1:14" ht="55.2">
       <c r="A27" t="s">
         <v>203</v>
       </c>
@@ -23608,11 +23608,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C27" s="240" t="str">
+      <c r="C27" s="216" t="str">
         <f>VLOOKUP(A27,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Phát nhạc dựa trên nhận diện cảm xúc trên khuôn mặt sử dụng Raspberry Pi 4</v>
       </c>
-      <c r="D27" s="240" t="str">
+      <c r="D27" s="216" t="str">
         <f>VLOOKUP(A27,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Phát nhạc dựa trên nhận diện cảm xúc trên khuôn mặt sử dụng Raspberry Pi 4</v>
       </c>
@@ -23647,7 +23647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="28">
+    <row r="28" spans="1:14" ht="27.6">
       <c r="A28" t="s">
         <v>207</v>
       </c>
@@ -23655,11 +23655,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C28" s="240" t="str">
+      <c r="C28" s="216" t="str">
         <f>VLOOKUP(A28,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Xây dựng hệ thống điểm danh sinh viên qua RFID</v>
       </c>
-      <c r="D28" s="240" t="str">
+      <c r="D28" s="216" t="str">
         <f>VLOOKUP(A28,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Xây dựng hệ thống điểm danh sinh viên qua RFID</v>
       </c>
@@ -23694,7 +23694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="42">
+    <row r="29" spans="1:14" ht="41.4">
       <c r="A29" t="s">
         <v>212</v>
       </c>
@@ -23702,11 +23702,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C29" s="240" t="str">
+      <c r="C29" s="216" t="str">
         <f>VLOOKUP(A29,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Giám sát và điều khiển mô hình nhà thông minh trên giao diện web</v>
       </c>
-      <c r="D29" s="240" t="str">
+      <c r="D29" s="216" t="str">
         <f>VLOOKUP(A29,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Giám sát và điều khiển mô hình nhà thông minh trên giao diện web</v>
       </c>
@@ -23714,7 +23714,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F29" s="240" t="s">
+      <c r="F29" s="216" t="s">
         <v>814</v>
       </c>
       <c r="G29" s="210" t="str">
@@ -23744,7 +23744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="56">
+    <row r="30" spans="1:14" ht="55.2">
       <c r="A30" t="s">
         <v>216</v>
       </c>
@@ -23752,11 +23752,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C30" s="240" t="str">
+      <c r="C30" s="216" t="str">
         <f>VLOOKUP(A30,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Xây dựng hệ thống quan trắc ứng dụng open source Grafana và Prometheus</v>
       </c>
-      <c r="D30" s="240" t="str">
+      <c r="D30" s="216" t="str">
         <f>VLOOKUP(A30,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Xây dựng hệ thống quan trắc ứng dụng open source Grafana và Prometheus</v>
       </c>
@@ -23791,7 +23791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="28">
+    <row r="31" spans="1:14" ht="27.6">
       <c r="A31" t="s">
         <v>221</v>
       </c>
@@ -23799,11 +23799,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C31" s="240" t="str">
+      <c r="C31" s="216" t="str">
         <f>VLOOKUP(A31,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Thiết kế và phát triển thiết bị bay Quadcopter</v>
       </c>
-      <c r="D31" s="240" t="str">
+      <c r="D31" s="216" t="str">
         <f>VLOOKUP(A31,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Thiết kế và phát triển thiết bị bay Quadcopter</v>
       </c>
@@ -23838,19 +23838,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="56">
-      <c r="A32" s="237" t="s">
+    <row r="32" spans="1:14" ht="55.2">
+      <c r="A32" s="213" t="s">
         <v>226</v>
       </c>
       <c r="B32" s="210">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C32" s="240" t="str">
+      <c r="C32" s="216" t="str">
         <f>VLOOKUP(A32,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Nghiên cứu phương pháp loại bỏ phản hồi âm thanh sử dụng bộ lọc thích nghi và ứng dụng</v>
       </c>
-      <c r="D32" s="240" t="str">
+      <c r="D32" s="216" t="str">
         <f>VLOOKUP(A32,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Nghiên cứu phương pháp loại bỏ phản hồi âm thanh sử dụng bộ lọc thích nghi và ứng dụng</v>
       </c>
@@ -23885,19 +23885,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="56">
-      <c r="A33" s="237" t="s">
+    <row r="33" spans="1:14" ht="55.2">
+      <c r="A33" s="213" t="s">
         <v>231</v>
       </c>
       <c r="B33" s="210">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C33" s="240" t="str">
+      <c r="C33" s="216" t="str">
         <f>VLOOKUP(A33,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Nghiên cứu phương pháp chống ồn chủ động sử dụng thuật toán thích nghi và ứng dụng</v>
       </c>
-      <c r="D33" s="240" t="str">
+      <c r="D33" s="216" t="str">
         <f>VLOOKUP(A33,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Nghiên cứu phương pháp chống ồn chủ động sử dụng thuật toán thích nghi và ứng dụng</v>
       </c>
@@ -23932,19 +23932,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="42">
-      <c r="A34" s="237" t="s">
+    <row r="34" spans="1:14" ht="41.4">
+      <c r="A34" s="213" t="s">
         <v>235</v>
       </c>
       <c r="B34" s="210">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C34" s="240" t="str">
+      <c r="C34" s="216" t="str">
         <f>VLOOKUP(A34,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Bãi đỗ xe thông minh tích hợp nhận diện biển số xe vào thẻ từ.</v>
       </c>
-      <c r="D34" s="240" t="str">
+      <c r="D34" s="216" t="str">
         <f>VLOOKUP(A34,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Bãi đỗ xe thông minh tích hợp nhận diện biển số xe vào thẻ từ.</v>
       </c>
@@ -23979,19 +23979,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="42">
-      <c r="A35" s="237" t="s">
+    <row r="35" spans="1:14" ht="41.4">
+      <c r="A35" s="213" t="s">
         <v>240</v>
       </c>
       <c r="B35" s="210">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C35" s="240" t="str">
+      <c r="C35" s="216" t="str">
         <f>VLOOKUP(A35,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Thiết kế, thử nghiệm ổ cắm thông minh điều khiển bằng giọng nói</v>
       </c>
-      <c r="D35" s="240" t="str">
+      <c r="D35" s="216" t="str">
         <f>VLOOKUP(A35,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Thiết kế, thử nghiệm ổ cắm thông minh điều khiển bằng giọng nói</v>
       </c>
@@ -24026,19 +24026,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="42">
-      <c r="A36" s="237" t="s">
+    <row r="36" spans="1:14" ht="41.4">
+      <c r="A36" s="213" t="s">
         <v>244</v>
       </c>
       <c r="B36" s="210">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C36" s="240" t="str">
+      <c r="C36" s="216" t="str">
         <f>VLOOKUP(A36,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Xây dựng hệ thống quan trắc khí tượng sử dụng nền tảng Grafana</v>
       </c>
-      <c r="D36" s="240" t="str">
+      <c r="D36" s="216" t="str">
         <f>VLOOKUP(A36,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Xây dựng hệ thống quan trắc khí tượng sử dụng nền tảng Grafana</v>
       </c>
@@ -24073,19 +24073,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="42">
-      <c r="A37" s="237" t="s">
+    <row r="37" spans="1:14" ht="55.2">
+      <c r="A37" s="213" t="s">
         <v>249</v>
       </c>
       <c r="B37" s="210">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C37" s="240" t="str">
+      <c r="C37" s="216" t="str">
         <f>VLOOKUP(A37,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Phát triển hệ thống đo lường, giám sát chất lượng không khí trong nhà</v>
       </c>
-      <c r="D37" s="240" t="str">
+      <c r="D37" s="216" t="str">
         <f>VLOOKUP(A37,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Phát triển hệ thống đo lường, giám sát chất lượng không khí trong nhà</v>
       </c>
@@ -24120,19 +24120,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="42">
-      <c r="A38" s="237" t="s">
+    <row r="38" spans="1:14" ht="41.4">
+      <c r="A38" s="213" t="s">
         <v>254</v>
       </c>
       <c r="B38" s="210">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C38" s="240" t="str">
+      <c r="C38" s="216" t="str">
         <f>VLOOKUP(A38,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Phát triển hệ thống đo lường và hiển thị chất lượng đất</v>
       </c>
-      <c r="D38" s="240" t="str">
+      <c r="D38" s="216" t="str">
         <f>VLOOKUP(A38,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Phát triển hệ thống đo lường và hiển thị chất lượng đất</v>
       </c>
@@ -24167,19 +24167,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="42">
-      <c r="A39" s="237" t="s">
+    <row r="39" spans="1:14" ht="41.4">
+      <c r="A39" s="213" t="s">
         <v>258</v>
       </c>
       <c r="B39" s="210">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C39" s="240" t="str">
+      <c r="C39" s="216" t="str">
         <f>VLOOKUP(A39,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Thiết kế máy bán hàng tự động sử dụng phương thức thanh toán QR code</v>
       </c>
-      <c r="D39" s="240" t="str">
+      <c r="D39" s="216" t="str">
         <f>VLOOKUP(A39,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Thiết kế máy bán hàng tự động sử dụng phương thức thanh toán QR code</v>
       </c>
@@ -24214,19 +24214,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="56">
-      <c r="A40" s="237" t="s">
+    <row r="40" spans="1:14" ht="55.2">
+      <c r="A40" s="213" t="s">
         <v>263</v>
       </c>
       <c r="B40" s="210">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C40" s="240" t="str">
+      <c r="C40" s="216" t="str">
         <f>VLOOKUP(A40,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Xây dựng mô hình mạng cảm biến để giám sát và điều khiển thiết bị điện trong nhà</v>
       </c>
-      <c r="D40" s="240" t="str">
+      <c r="D40" s="216" t="str">
         <f>VLOOKUP(A40,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Xây dựng mô hình mạng cảm biến để giám sát và điều khiển thiết bị điện trong nhà</v>
       </c>
@@ -24261,19 +24261,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="42">
-      <c r="A41" s="237" t="s">
+    <row r="41" spans="1:14" ht="41.4">
+      <c r="A41" s="213" t="s">
         <v>268</v>
       </c>
       <c r="B41" s="210">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C41" s="240" t="str">
+      <c r="C41" s="216" t="str">
         <f>VLOOKUP(A41,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Xây dựng hệ thống phân loại và quản lý sản phẩm bằng mã QR</v>
       </c>
-      <c r="D41" s="240" t="str">
+      <c r="D41" s="216" t="str">
         <f>VLOOKUP(A41,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Xây dựng hệ thống phân loại và quản lý sản phẩm bằng mã QR</v>
       </c>
@@ -24281,7 +24281,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F41" s="240" t="s">
+      <c r="F41" s="216" t="s">
         <v>814</v>
       </c>
       <c r="G41" s="210" t="str">
@@ -24311,19 +24311,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="42">
-      <c r="A42" s="237" t="s">
+    <row r="42" spans="1:14" ht="41.4">
+      <c r="A42" s="213" t="s">
         <v>273</v>
       </c>
       <c r="B42" s="210">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C42" s="240" t="str">
+      <c r="C42" s="216" t="str">
         <f>VLOOKUP(A42,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Xây hệ thống giám sát và cảnh báo cháy và rò rỉ khí gas cho nhà thông minh</v>
       </c>
-      <c r="D42" s="240" t="str">
+      <c r="D42" s="216" t="str">
         <f>VLOOKUP(A42,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>xây hệ thống giám sát và cảnh báo cháy và rò rỉ khí gas cho nhà thông minh</v>
       </c>
@@ -24358,19 +24358,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="28">
-      <c r="A43" s="237" t="s">
+    <row r="43" spans="1:14" ht="27.6">
+      <c r="A43" s="213" t="s">
         <v>277</v>
       </c>
       <c r="B43" s="210">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C43" s="240" t="str">
+      <c r="C43" s="216" t="str">
         <f>VLOOKUP(A43,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Nghiên cứu xây dựng bãi đỗ xe thông minh</v>
       </c>
-      <c r="D43" s="240" t="str">
+      <c r="D43" s="216" t="str">
         <f>VLOOKUP(A43,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Nghiên cứu xây dựng bãi đỗ xe thông minh</v>
       </c>
@@ -24405,19 +24405,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="28">
-      <c r="A44" s="237" t="s">
+    <row r="44" spans="1:14" ht="27.6">
+      <c r="A44" s="213" t="s">
         <v>281</v>
       </c>
       <c r="B44" s="210">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C44" s="240" t="str">
+      <c r="C44" s="216" t="str">
         <f>VLOOKUP(A44,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Cánh tay robot sắp xếp hàng hóa</v>
       </c>
-      <c r="D44" s="240" t="str">
+      <c r="D44" s="216" t="str">
         <f>VLOOKUP(A44,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Cánh tay robot sắp xếp hàng hóa</v>
       </c>
@@ -24452,19 +24452,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="28">
-      <c r="A45" s="237" t="s">
+    <row r="45" spans="1:14" ht="27.6">
+      <c r="A45" s="213" t="s">
         <v>285</v>
       </c>
       <c r="B45" s="210">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C45" s="240" t="str">
+      <c r="C45" s="216" t="str">
         <f>VLOOKUP(A45,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Hệ thống báo cháy thông minh</v>
       </c>
-      <c r="D45" s="240" t="str">
+      <c r="D45" s="216" t="str">
         <f>VLOOKUP(A45,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Hệ thống báo cháy thông minh</v>
       </c>
@@ -24472,7 +24472,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F45" s="240" t="s">
+      <c r="F45" s="216" t="s">
         <v>814</v>
       </c>
       <c r="G45" s="210" t="str">
@@ -24502,19 +24502,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="28">
-      <c r="A46" s="237" t="s">
+    <row r="46" spans="1:14" ht="27.6">
+      <c r="A46" s="213" t="s">
         <v>289</v>
       </c>
       <c r="B46" s="210">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C46" s="240" t="str">
+      <c r="C46" s="216" t="str">
         <f>VLOOKUP(A46,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Thiết kế hệ thống bãi đỗ xe thông minh</v>
       </c>
-      <c r="D46" s="240" t="str">
+      <c r="D46" s="216" t="str">
         <f>VLOOKUP(A46,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Thiết kế hệ thống bãi đỗ xe thông minh</v>
       </c>
@@ -24549,19 +24549,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="42">
-      <c r="A47" s="237" t="s">
+    <row r="47" spans="1:14" ht="41.4">
+      <c r="A47" s="213" t="s">
         <v>294</v>
       </c>
       <c r="B47" s="210">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C47" s="240" t="str">
+      <c r="C47" s="216" t="str">
         <f>VLOOKUP(A47,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Thiết kế và phát triển hệ thống cảnh báo rò rỉ khí gas</v>
       </c>
-      <c r="D47" s="240" t="str">
+      <c r="D47" s="216" t="str">
         <f>VLOOKUP(A47,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Thiết kế và phát triển hệ thống cảnh báo rò rỉ khí gas</v>
       </c>
@@ -24596,7 +24596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="42">
+    <row r="48" spans="1:14" ht="55.2">
       <c r="A48" t="s">
         <v>298</v>
       </c>
@@ -24604,11 +24604,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C48" s="240" t="str">
+      <c r="C48" s="216" t="str">
         <f>VLOOKUP(A48,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Xây dựng bản đồ và hệ thống giám sát môi trường cho xe tự hành</v>
       </c>
-      <c r="D48" s="240" t="str">
+      <c r="D48" s="216" t="str">
         <f>VLOOKUP(A48,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Xây dựng bản đồ và hệ thống giám sát môi trường cho xe tự hành</v>
       </c>
@@ -24616,7 +24616,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F48" s="240" t="s">
+      <c r="F48" s="216" t="s">
         <v>815</v>
       </c>
       <c r="G48" s="210" t="str">
@@ -24646,7 +24646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="42">
+    <row r="49" spans="1:14" ht="55.2">
       <c r="A49" t="s">
         <v>302</v>
       </c>
@@ -24654,11 +24654,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C49" s="240" t="str">
+      <c r="C49" s="216" t="str">
         <f>VLOOKUP(A49,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Nhận dạng và bóc tách văn bản nhờ kỹ thuật nhận dạng quang học OCR</v>
       </c>
-      <c r="D49" s="240" t="str">
+      <c r="D49" s="216" t="str">
         <f>VLOOKUP(A49,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Nhận dạng và bóc tách văn bản nhờ kỹ thuật nhận dạng quang học OCR</v>
       </c>
@@ -24693,7 +24693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="56">
+    <row r="50" spans="1:14" ht="55.2">
       <c r="A50" t="s">
         <v>306</v>
       </c>
@@ -24701,11 +24701,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C50" s="240" t="str">
+      <c r="C50" s="216" t="str">
         <f>VLOOKUP(A50,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Xây dựng hệ thống bãi đỗ xe thông minh và tự động thông báo chỉ dẫn đường đi</v>
       </c>
-      <c r="D50" s="240" t="str">
+      <c r="D50" s="216" t="str">
         <f>VLOOKUP(A50,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Xây dựng hệ thống bãi đỗ xe thông minh và tự động thông báo chỉ dẫn đường đi</v>
       </c>
@@ -24740,7 +24740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="42">
+    <row r="51" spans="1:14" ht="41.4">
       <c r="A51" t="s">
         <v>310</v>
       </c>
@@ -24748,11 +24748,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C51" s="240" t="str">
+      <c r="C51" s="216" t="str">
         <f>VLOOKUP(A51,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Hệ thống điều khiển nhà cho người khiếm khuyết bằng giọng nói và cử chỉ</v>
       </c>
-      <c r="D51" s="240" t="str">
+      <c r="D51" s="216" t="str">
         <f>VLOOKUP(A51,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Hệ thống điều khiển nhà cho người khiếm khuyết bằng giọng nói và cử chỉ</v>
       </c>
@@ -24787,7 +24787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="42">
+    <row r="52" spans="1:14" ht="41.4">
       <c r="A52" t="s">
         <v>315</v>
       </c>
@@ -24795,11 +24795,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C52" s="240" t="str">
+      <c r="C52" s="216" t="str">
         <f>VLOOKUP(A52,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Xây dựng hệ thống băng truyền phân loại sản phẩm dựa vào màu sắc</v>
       </c>
-      <c r="D52" s="240" t="str">
+      <c r="D52" s="216" t="str">
         <f>VLOOKUP(A52,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Xây dựng hệ thống băng truyền phân loại sản phẩm dựa vào màu sắc</v>
       </c>
@@ -24834,7 +24834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="42">
+    <row r="53" spans="1:14" ht="41.4">
       <c r="A53" t="s">
         <v>320</v>
       </c>
@@ -24842,11 +24842,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C53" s="240" t="str">
+      <c r="C53" s="216" t="str">
         <f>VLOOKUP(A53,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Hệ thống IoT giám sát môi trường và phòng chống cháy nổ cho nhà ở</v>
       </c>
-      <c r="D53" s="240" t="str">
+      <c r="D53" s="216" t="str">
         <f>VLOOKUP(A53,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Hệ thống IoT giám sát môi trường và phòng chống cháy nổ cho nhà ở</v>
       </c>
@@ -24881,7 +24881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="28">
+    <row r="54" spans="1:14" ht="27.6">
       <c r="A54" t="s">
         <v>325</v>
       </c>
@@ -24889,11 +24889,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C54" s="240" t="str">
+      <c r="C54" s="216" t="str">
         <f>VLOOKUP(A54,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Xây dựng hệ thống điều khiển IoT bằng giọng nói</v>
       </c>
-      <c r="D54" s="240" t="str">
+      <c r="D54" s="216" t="str">
         <f>VLOOKUP(A54,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Xây dựng hệ thống điều khiển IoT bằng giọng nói</v>
       </c>
@@ -24928,7 +24928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="42">
+    <row r="55" spans="1:14" ht="41.4">
       <c r="A55" t="s">
         <v>328</v>
       </c>
@@ -24936,11 +24936,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C55" s="240" t="str">
+      <c r="C55" s="216" t="str">
         <f>VLOOKUP(A55,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Thiết kế hệ thống giám sát sức khỏe sử dụng giao tiếp CoAP</v>
       </c>
-      <c r="D55" s="240" t="str">
+      <c r="D55" s="216" t="str">
         <f>VLOOKUP(A55,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Thiết kế hệ thống giám sát sức khỏe sử dụng giao tiếp CoAP</v>
       </c>
@@ -24975,7 +24975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="42">
+    <row r="56" spans="1:14" ht="55.2">
       <c r="A56" t="s">
         <v>331</v>
       </c>
@@ -24983,11 +24983,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C56" s="240" t="str">
+      <c r="C56" s="216" t="str">
         <f>VLOOKUP(A56,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Nhận dạng và bóc tách văn bản nhờ kỹ thuật nhận dạng quang học OCR. </v>
       </c>
-      <c r="D56" s="240" t="str">
+      <c r="D56" s="216" t="str">
         <f>VLOOKUP(A56,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Nhận dạng và bóc tách văn bản nhờ kỹ thuật nhận dạng quang học OCR. </v>
       </c>
@@ -25022,7 +25022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="42">
+    <row r="57" spans="1:14" ht="41.4">
       <c r="A57" t="s">
         <v>334</v>
       </c>
@@ -25030,11 +25030,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C57" s="240" t="str">
+      <c r="C57" s="216" t="str">
         <f>VLOOKUP(A57,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Thiết kế mạch IOT quản lý chất lượng nước lại hồ nuôi tôm cá</v>
       </c>
-      <c r="D57" s="240" t="str">
+      <c r="D57" s="216" t="str">
         <f>VLOOKUP(A57,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Thiết kế mạch IOT quản lý chất lượng nước lại hồ nuôi tôm cá</v>
       </c>
@@ -25069,7 +25069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="42">
+    <row r="58" spans="1:14" ht="41.4">
       <c r="A58" t="s">
         <v>338</v>
       </c>
@@ -25077,11 +25077,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C58" s="240" t="str">
+      <c r="C58" s="216" t="str">
         <f>VLOOKUP(A58,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Giám sát và quản lí các thiết bị điện trong nhà thông qua trợ lí ảo</v>
       </c>
-      <c r="D58" s="240" t="str">
+      <c r="D58" s="216" t="str">
         <f>VLOOKUP(A58,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Giám sát và quản lí các thiết bị điện trong nhà thông qua trợ lí ảo</v>
       </c>
@@ -25116,7 +25116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="42">
+    <row r="59" spans="1:14" ht="41.4">
       <c r="A59" t="s">
         <v>343</v>
       </c>
@@ -25124,11 +25124,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C59" s="240" t="str">
+      <c r="C59" s="216" t="str">
         <f>VLOOKUP(A59,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Thiết kế và phát triển hệ thống IoT giám sát sức khỏe</v>
       </c>
-      <c r="D59" s="240" t="str">
+      <c r="D59" s="216" t="str">
         <f>VLOOKUP(A59,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Thiết kế và phát triển hệ thống IoT giám sát sức khỏe</v>
       </c>
@@ -25163,7 +25163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="42">
+    <row r="60" spans="1:14" ht="41.4">
       <c r="A60" t="s">
         <v>348</v>
       </c>
@@ -25171,11 +25171,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C60" s="240" t="str">
+      <c r="C60" s="216" t="str">
         <f>VLOOKUP(A60,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Xây dựng nhà thông minh sử dụng  Arduino Uno và ESP32 CAM</v>
       </c>
-      <c r="D60" s="240" t="str">
+      <c r="D60" s="216" t="str">
         <f>VLOOKUP(A60,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Xây dựng nhà thông minh sử dụng  Arduino Uno và ESP32 CAM</v>
       </c>
@@ -25210,7 +25210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="28">
+    <row r="61" spans="1:14" ht="27.6">
       <c r="A61" t="s">
         <v>352</v>
       </c>
@@ -25218,11 +25218,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C61" s="240" t="str">
+      <c r="C61" s="216" t="str">
         <f>VLOOKUP(A61,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Xây dựng bộ thiết bị theo dõi và giám sát nhà từ xa</v>
       </c>
-      <c r="D61" s="240" t="str">
+      <c r="D61" s="216" t="str">
         <f>VLOOKUP(A61,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Xây dựng bộ thiết bị theo dõi và giám sát nhà từ xa</v>
       </c>
@@ -25257,7 +25257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="42">
+    <row r="62" spans="1:14" ht="41.4">
       <c r="A62" t="s">
         <v>356</v>
       </c>
@@ -25265,11 +25265,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C62" s="240" t="str">
+      <c r="C62" s="216" t="str">
         <f>VLOOKUP(A62,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Phát triển hệ thống IoT cho nông nghiệp sử dụng Raspberry Pi và Coze AI</v>
       </c>
-      <c r="D62" s="240" t="str">
+      <c r="D62" s="216" t="str">
         <f>VLOOKUP(A62,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Phát triển hệ thống IoT cho nông nghiệp sử dụng Raspberry Pi và Coze AI</v>
       </c>
@@ -25304,7 +25304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="42">
+    <row r="63" spans="1:14" ht="41.4">
       <c r="A63" t="s">
         <v>359</v>
       </c>
@@ -25312,11 +25312,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C63" s="240" t="str">
+      <c r="C63" s="216" t="str">
         <f>VLOOKUP(A63,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Xây dựng hệ thống đèn đường dựa trên mạng LoRa Mesh</v>
       </c>
-      <c r="D63" s="240" t="str">
+      <c r="D63" s="216" t="str">
         <f>VLOOKUP(A63,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Xây dựng hệ thống đèn đường dựa trên mạng LoRa Mesh</v>
       </c>
@@ -25351,19 +25351,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="70">
-      <c r="A64" s="238" t="s">
+    <row r="64" spans="1:14" ht="69">
+      <c r="A64" s="214" t="s">
         <v>362</v>
       </c>
       <c r="B64" s="210">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C64" s="240" t="str">
+      <c r="C64" s="216" t="str">
         <f>VLOOKUP(A64,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Thiết kế và mô phỏng hệ thống truyền tin đơn giản ứng dụng mã kiểm tra và sửa lỗi Hamming trên FPGA</v>
       </c>
-      <c r="D64" s="240" t="str">
+      <c r="D64" s="216" t="str">
         <f>VLOOKUP(A64,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Thiết kế và mô phỏng hệ thống truyền tin đơn giản ứng dụng mã kiểm tra và sửa lỗi Hamming trên FPGA</v>
       </c>
@@ -25371,7 +25371,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F64" s="240" t="s">
+      <c r="F64" s="216" t="s">
         <v>814</v>
       </c>
       <c r="G64" s="210" t="str">
@@ -25401,19 +25401,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="70">
-      <c r="A65" s="238" t="s">
+    <row r="65" spans="1:14" ht="69">
+      <c r="A65" s="214" t="s">
         <v>365</v>
       </c>
       <c r="B65" s="210">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C65" s="240" t="str">
+      <c r="C65" s="216" t="str">
         <f>VLOOKUP(A65,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Mô phỏng và thiết kế bộ truyền tin đơn giản ứng dụng mã phát hiện và sửa sai Reed Solomon trên FPGA</v>
       </c>
-      <c r="D65" s="240" t="str">
+      <c r="D65" s="216" t="str">
         <f>VLOOKUP(A65,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Mô phỏng và thiết kế bộ truyền tin đơn giản ứng dụng mã phát hiện và sửa sai Reed Solomon trên FPGA</v>
       </c>
@@ -25421,7 +25421,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F65" s="240" t="s">
+      <c r="F65" s="216" t="s">
         <v>814</v>
       </c>
       <c r="G65" s="210" t="str">
@@ -25451,19 +25451,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="42">
-      <c r="A66" s="238" t="s">
+    <row r="66" spans="1:14" ht="41.4">
+      <c r="A66" s="214" t="s">
         <v>370</v>
       </c>
       <c r="B66" s="210">
         <f t="shared" ref="B66:B107" si="4">VLOOKUP(A66,$K$1:$L$189,2,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="C66" s="240" t="str">
+      <c r="C66" s="216" t="str">
         <f>VLOOKUP(A66,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Nghiên cứu, mô phỏng các bộ lọc thích nghi sử dụng Matlab</v>
       </c>
-      <c r="D66" s="240" t="str">
+      <c r="D66" s="216" t="str">
         <f>VLOOKUP(A66,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Nghiên cứu, mô phỏng các bộ lọc thích nghi sử dụng Matlab</v>
       </c>
@@ -25498,19 +25498,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:14" ht="56">
-      <c r="A67" s="238" t="s">
+    <row r="67" spans="1:14" ht="55.2">
+      <c r="A67" s="214" t="s">
         <v>373</v>
       </c>
       <c r="B67" s="210">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="C67" s="240" t="str">
+      <c r="C67" s="216" t="str">
         <f>VLOOKUP(A67,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Nghiên cứu, mô phỏng các phương pháp mã hóa tiếng nói tốc độ thấp sử dụng Matlab</v>
       </c>
-      <c r="D67" s="240" t="str">
+      <c r="D67" s="216" t="str">
         <f>VLOOKUP(A67,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Nghiên cứu, mô phỏng các phương pháp mã hóa tiếng nói tốc độ thấp sử dụng Matlab</v>
       </c>
@@ -25545,19 +25545,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:14" ht="56">
-      <c r="A68" s="238" t="s">
+    <row r="68" spans="1:14" ht="55.2">
+      <c r="A68" s="214" t="s">
         <v>377</v>
       </c>
       <c r="B68" s="210">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="C68" s="240" t="str">
+      <c r="C68" s="216" t="str">
         <f>VLOOKUP(A68,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Nghiên cứu các giải pháp thu thập năng lượng từ sóng vô tuyến cho các thiết bị IoT</v>
       </c>
-      <c r="D68" s="240" t="str">
+      <c r="D68" s="216" t="str">
         <f>VLOOKUP(A68,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Nghiên cứu các giải pháp thu thập năng lượng từ sóng vô tuyến cho các thiết bị IoT</v>
       </c>
@@ -25592,19 +25592,19 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="42">
-      <c r="A69" s="238" t="s">
+    <row r="69" spans="1:14" ht="41.4">
+      <c r="A69" s="214" t="s">
         <v>381</v>
       </c>
       <c r="B69" s="210">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="C69" s="240" t="str">
+      <c r="C69" s="216" t="str">
         <f>VLOOKUP(A69,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Xây dựng hề thống tự động phân loại sản phẩm ứng dụng camera AI</v>
       </c>
-      <c r="D69" s="240" t="str">
+      <c r="D69" s="216" t="str">
         <f>VLOOKUP(A69,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Xây dựng hề thống tự động phân loại sản phẩm ứng dụng camera AI</v>
       </c>
@@ -25639,19 +25639,19 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="56">
-      <c r="A70" s="238" t="s">
+    <row r="70" spans="1:14" ht="55.2">
+      <c r="A70" s="214" t="s">
         <v>384</v>
       </c>
       <c r="B70" s="210">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="C70" s="240" t="str">
+      <c r="C70" s="216" t="str">
         <f>VLOOKUP(A70,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Xây dựng hệ thống IoT giám sát và điều khiển nồng độ khí CO2 trong tòa nhà làm việc công sở</v>
       </c>
-      <c r="D70" s="240" t="str">
+      <c r="D70" s="216" t="str">
         <f>VLOOKUP(A70,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Xây dựng hệ thống IoT giám sát và điều khiển nồng độ khí CO2 trong tòa nhà làm việc công sở</v>
       </c>
@@ -25686,19 +25686,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:14" ht="28">
-      <c r="A71" s="238" t="s">
+    <row r="71" spans="1:14" ht="27.6">
+      <c r="A71" s="214" t="s">
         <v>387</v>
       </c>
       <c r="B71" s="210">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="C71" s="240" t="str">
+      <c r="C71" s="216" t="str">
         <f>VLOOKUP(A71,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v xml:space="preserve">Thiết kế bộ khuyếch đại vì sai folded cascode </v>
       </c>
-      <c r="D71" s="240" t="str">
+      <c r="D71" s="216" t="str">
         <f>VLOOKUP(A71,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v xml:space="preserve">Thiết kế bộ khuyếch đại vì sai folded cascode </v>
       </c>
@@ -25733,19 +25733,19 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="56">
-      <c r="A72" s="238" t="s">
+    <row r="72" spans="1:14" ht="69">
+      <c r="A72" s="214" t="s">
         <v>390</v>
       </c>
       <c r="B72" s="210">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="C72" s="240" t="str">
+      <c r="C72" s="216" t="str">
         <f>VLOOKUP(A72,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Nghiên cứu, xây dựng thiết bị đọc cảm biến nhiệt độ Thermocouple và điều khiển Relay bán dẫn.</v>
       </c>
-      <c r="D72" s="240" t="str">
+      <c r="D72" s="216" t="str">
         <f>VLOOKUP(A72,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Nghiên cứu, xây dựng thiết bị đọc cảm biến nhiệt độ Thermocouple và điều khiển Relay bán dẫn.</v>
       </c>
@@ -25780,19 +25780,19 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="73" spans="1:14" ht="42">
-      <c r="A73" s="238" t="s">
+    <row r="73" spans="1:14" ht="41.4">
+      <c r="A73" s="214" t="s">
         <v>394</v>
       </c>
       <c r="B73" s="210">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="C73" s="240" t="str">
+      <c r="C73" s="216" t="str">
         <f>VLOOKUP(A73,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Nghiên cứu các thuật toán tối ưu trong thiết kế vật lý và ứng dụng</v>
       </c>
-      <c r="D73" s="240" t="str">
+      <c r="D73" s="216" t="str">
         <f>VLOOKUP(A73,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Nghiên cứu các thuật toán tối ưu trong thiết kế vật lý và ứng dụng</v>
       </c>
@@ -25827,19 +25827,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:14" ht="98">
-      <c r="A74" s="238" t="s">
+    <row r="74" spans="1:14" ht="96.6">
+      <c r="A74" s="214" t="s">
         <v>399</v>
       </c>
       <c r="B74" s="210">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="C74" s="240" t="str">
+      <c r="C74" s="216" t="str">
         <f>VLOOKUP(A74,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Thiết kê mô hình RTL và kiểm thử UVM cho giao tiếp AHB-APB (RTL Design and UVM Verification for AHB_APB_bridge protocol)</v>
       </c>
-      <c r="D74" s="240" t="str">
+      <c r="D74" s="216" t="str">
         <f>VLOOKUP(A74,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Thiết kê mô hình RTL và kiểm thử UVM cho giao tiếp AHB-APB (RTL Design and UVM Verification for AHB_APB_bridge protocol)</v>
       </c>
@@ -25874,19 +25874,19 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="75" spans="1:14" ht="42">
-      <c r="A75" s="238" t="s">
+    <row r="75" spans="1:14" ht="41.4">
+      <c r="A75" s="214" t="s">
         <v>404</v>
       </c>
       <c r="B75" s="210">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="C75" s="240" t="str">
+      <c r="C75" s="216" t="str">
         <f>VLOOKUP(A75,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Xây dựng hệ thống xác thực dữ liệu sử dụng FPGA</v>
       </c>
-      <c r="D75" s="240" t="str">
+      <c r="D75" s="216" t="str">
         <f>VLOOKUP(A75,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Xây dựng hệ thống xác thực dữ liệu sử dụng FPGA</v>
       </c>
@@ -25921,19 +25921,19 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="76" spans="1:14" ht="42">
-      <c r="A76" s="238" t="s">
+    <row r="76" spans="1:14" ht="41.4">
+      <c r="A76" s="214" t="s">
         <v>406</v>
       </c>
       <c r="B76" s="210">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="C76" s="240" t="str">
+      <c r="C76" s="216" t="str">
         <f>VLOOKUP(A76,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Nghiên cứu và xây dựng cân tính tiền thông minh sử dụng Raspberry Pi</v>
       </c>
-      <c r="D76" s="240" t="str">
+      <c r="D76" s="216" t="str">
         <f>VLOOKUP(A76,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Nghiên cứu và xây dựng cân tính tiền thông minh sử dụng Raspberry Pi</v>
       </c>
@@ -25968,19 +25968,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:14" ht="56">
-      <c r="A77" s="238" t="s">
+    <row r="77" spans="1:14" ht="55.2">
+      <c r="A77" s="214" t="s">
         <v>410</v>
       </c>
       <c r="B77" s="210">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="C77" s="240" t="str">
+      <c r="C77" s="216" t="str">
         <f>VLOOKUP(A77,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Nghiên cứu và xây dựng màn hình điều khiển các thiết bị trong gia đình sử dụng Raspberry Pi 4</v>
       </c>
-      <c r="D77" s="240" t="str">
+      <c r="D77" s="216" t="str">
         <f>VLOOKUP(A77,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Nghiên cứu và xây dựng màn hình điều khiển các thiết bị trong gia đình sử dụng Raspberry Pi 4</v>
       </c>
@@ -26015,19 +26015,19 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="78" spans="1:14" ht="28">
-      <c r="A78" s="238" t="s">
+    <row r="78" spans="1:14" ht="27.6">
+      <c r="A78" s="214" t="s">
         <v>414</v>
       </c>
       <c r="B78" s="210">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="C78" s="240" t="str">
+      <c r="C78" s="216" t="str">
         <f>VLOOKUP(A78,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Thiết kế bộ vi xử lý RISC-V bằng ngôn ngữ Verilog</v>
       </c>
-      <c r="D78" s="240" t="str">
+      <c r="D78" s="216" t="str">
         <f>VLOOKUP(A78,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Thiết kế bộ vi xử lý RISC-V bằng ngôn ngữ Verilog</v>
       </c>
@@ -26062,7 +26062,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="79" spans="1:14" ht="28">
+    <row r="79" spans="1:14" ht="27.6">
       <c r="A79" t="s">
         <v>419</v>
       </c>
@@ -26070,11 +26070,11 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="C79" s="240" t="str">
+      <c r="C79" s="216" t="str">
         <f>VLOOKUP(A79,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Xe điều khiển tích hợp camera</v>
       </c>
-      <c r="D79" s="240" t="str">
+      <c r="D79" s="216" t="str">
         <f>VLOOKUP(A79,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Xe điều khiển tích hợp camera</v>
       </c>
@@ -26109,7 +26109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:14" ht="28">
+    <row r="80" spans="1:14" ht="27.6">
       <c r="A80" t="s">
         <v>424</v>
       </c>
@@ -26117,11 +26117,11 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="C80" s="240" t="str">
+      <c r="C80" s="216" t="str">
         <f>VLOOKUP(A80,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Cánh tay máy Robot vẽ tranh</v>
       </c>
-      <c r="D80" s="240" t="str">
+      <c r="D80" s="216" t="str">
         <f>VLOOKUP(A80,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Cánh tay máy Robot vẽ tranh</v>
       </c>
@@ -26156,7 +26156,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="81" spans="1:14" ht="28">
+    <row r="81" spans="1:14" ht="27.6">
       <c r="A81" t="s">
         <v>428</v>
       </c>
@@ -26164,11 +26164,11 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="C81" s="240" t="str">
+      <c r="C81" s="216" t="str">
         <f>VLOOKUP(A81,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Thiết kế xe tự hành dựa trên ROS2</v>
       </c>
-      <c r="D81" s="240" t="str">
+      <c r="D81" s="216" t="str">
         <f>VLOOKUP(A81,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Thiết kế xe tự hành dựa trên ROS2</v>
       </c>
@@ -26203,7 +26203,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="82" spans="1:14" ht="70">
+    <row r="82" spans="1:14" ht="69">
       <c r="A82" t="s">
         <v>433</v>
       </c>
@@ -26211,11 +26211,11 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="C82" s="240" t="str">
+      <c r="C82" s="216" t="str">
         <f>VLOOKUP(A82,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>MÔ HÌNH BĂNG TRUYỀN PHÂN LOẠI HÀNG HÓA DỰA TRÊN MÃ QR CODE HOẶC MÃ VẠCH</v>
       </c>
-      <c r="D82" s="240" t="str">
+      <c r="D82" s="216" t="str">
         <f>VLOOKUP(A82,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>MÔ HÌNH BĂNG TRUYỀN PHÂN LOẠI HÀNG HÓA DỰA TRÊN MÃ QR CODE HOẶC MÃ VẠCH</v>
       </c>
@@ -26250,7 +26250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:14" ht="42">
+    <row r="83" spans="1:14" ht="41.4">
       <c r="A83" t="s">
         <v>436</v>
       </c>
@@ -26258,11 +26258,11 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="C83" s="240" t="str">
+      <c r="C83" s="216" t="str">
         <f>VLOOKUP(A83,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Ứng dụng Keyword spotting trong điều khiển nhà thông minh</v>
       </c>
-      <c r="D83" s="240" t="str">
+      <c r="D83" s="216" t="str">
         <f>VLOOKUP(A83,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Ứng dụng Keyword spotting trong điều khiển nhà thông minh</v>
       </c>
@@ -26297,7 +26297,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="84" spans="1:14" ht="56">
+    <row r="84" spans="1:14" ht="55.2">
       <c r="A84" t="s">
         <v>438</v>
       </c>
@@ -26305,11 +26305,11 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="C84" s="240" t="str">
+      <c r="C84" s="216" t="str">
         <f>VLOOKUP(A84,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Xây dựng Smart Home dựa trên nền tảng ESP RainMaker kết hợp Voice Assistant</v>
       </c>
-      <c r="D84" s="240" t="str">
+      <c r="D84" s="216" t="str">
         <f>VLOOKUP(A84,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Xây dựng Smart Home dựa trên nền tảng ESP RainMaker kết hợp Voice Assistant</v>
       </c>
@@ -26344,7 +26344,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="85" spans="1:14" ht="42">
+    <row r="85" spans="1:14" ht="41.4">
       <c r="A85" t="s">
         <v>443</v>
       </c>
@@ -26352,11 +26352,11 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="C85" s="240" t="str">
+      <c r="C85" s="216" t="str">
         <f>VLOOKUP(A85,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Phát triển hệ thống giám sát và quản lý pin ứng dụng Edge Computing</v>
       </c>
-      <c r="D85" s="240" t="str">
+      <c r="D85" s="216" t="str">
         <f>VLOOKUP(A85,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Phát triển hệ thống giám sát và quản lý pin ứng dụng Edge Computing</v>
       </c>
@@ -26391,7 +26391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:14" ht="70">
+    <row r="86" spans="1:14" ht="69">
       <c r="A86" t="s">
         <v>447</v>
       </c>
@@ -26399,11 +26399,11 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="C86" s="240" t="str">
+      <c r="C86" s="216" t="str">
         <f>VLOOKUP(A86,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Xây dựng hệ thống IoT trong giám sát và điều khiển hệ thống pin năng lượng mặt trời công suất nhỏ</v>
       </c>
-      <c r="D86" s="240" t="str">
+      <c r="D86" s="216" t="str">
         <f>VLOOKUP(A86,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Xây dựng hệ thống IoT trong giám sát và điều khiển hệ thống pin năng lượng mặt trời công suất nhỏ</v>
       </c>
@@ -26438,7 +26438,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="87" spans="1:14" ht="42">
+    <row r="87" spans="1:14" ht="41.4">
       <c r="A87" t="s">
         <v>453</v>
       </c>
@@ -26446,11 +26446,11 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="C87" s="240" t="str">
+      <c r="C87" s="216" t="str">
         <f>VLOOKUP(A87,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Xây dựng ứng dụng IOT: Trạm quan trắc và cảnh báo thời tiết</v>
       </c>
-      <c r="D87" s="240" t="str">
+      <c r="D87" s="216" t="str">
         <f>VLOOKUP(A87,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Xây dựng ứng dụng IOT: Trạm quan trắc và cảnh báo thời tiết</v>
       </c>
@@ -26485,7 +26485,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="88" spans="1:14" ht="56">
+    <row r="88" spans="1:14" ht="55.2">
       <c r="A88" t="s">
         <v>456</v>
       </c>
@@ -26493,11 +26493,11 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="C88" s="240" t="str">
+      <c r="C88" s="216" t="str">
         <f>VLOOKUP(A88,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Thiết kế, xây dựng dây chuyền tự động phân loại sản phẩm và quản lý hàng hóa trực tuyến</v>
       </c>
-      <c r="D88" s="240" t="str">
+      <c r="D88" s="216" t="str">
         <f>VLOOKUP(A88,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Thiết kế, xây dựng dây chuyền tự động phân loại sản phẩm và quản lý hàng hóa trực tuyến</v>
       </c>
@@ -26532,7 +26532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:14" ht="42">
+    <row r="89" spans="1:14" ht="41.4">
       <c r="A89" t="s">
         <v>460</v>
       </c>
@@ -26540,11 +26540,11 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="C89" s="240" t="str">
+      <c r="C89" s="216" t="str">
         <f>VLOOKUP(A89,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Thiết kế thử nghiệm đồng hồ thông minh trên nền tảng Rain Maker</v>
       </c>
-      <c r="D89" s="240" t="str">
+      <c r="D89" s="216" t="str">
         <f>VLOOKUP(A89,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Thiết kế thử nghiệm đồng hồ thông minh trên nền tảng Rain Maker</v>
       </c>
@@ -26579,7 +26579,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="90" spans="1:14" ht="56">
+    <row r="90" spans="1:14" ht="55.2">
       <c r="A90" t="s">
         <v>463</v>
       </c>
@@ -26587,11 +26587,11 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="C90" s="240" t="str">
+      <c r="C90" s="216" t="str">
         <f>VLOOKUP(A90,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Xây dựng ứng dụng IOT: bộ điều khiển tập trung trong mô hình nhà thông minh</v>
       </c>
-      <c r="D90" s="240" t="str">
+      <c r="D90" s="216" t="str">
         <f>VLOOKUP(A90,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Xây dựng ứng dụng IOT: bộ điều khiển tập trung trong mô hình nhà thông minh</v>
       </c>
@@ -26626,7 +26626,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="91" spans="1:14" ht="42">
+    <row r="91" spans="1:14" ht="41.4">
       <c r="A91" t="s">
         <v>467</v>
       </c>
@@ -26634,11 +26634,11 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="C91" s="240" t="str">
+      <c r="C91" s="216" t="str">
         <f>VLOOKUP(A91,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Xây dựng mô hình IOT giám sát và điều khiển môi trường vườn</v>
       </c>
-      <c r="D91" s="240" t="str">
+      <c r="D91" s="216" t="str">
         <f>VLOOKUP(A91,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Xây dựng mô hình IOT giám sát và điều khiển môi trường vườn</v>
       </c>
@@ -26673,7 +26673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:14" ht="42">
+    <row r="92" spans="1:14" ht="41.4">
       <c r="A92" t="s">
         <v>471</v>
       </c>
@@ -26681,11 +26681,11 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="C92" s="240" t="str">
+      <c r="C92" s="216" t="str">
         <f>VLOOKUP(A92,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Hệ thống giám sát chất lượng không khí và điều khiển thiết bị qua Internet</v>
       </c>
-      <c r="D92" s="240" t="str">
+      <c r="D92" s="216" t="str">
         <f>VLOOKUP(A92,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Hệ thống giám sát chất lượng không khí và điều khiển thiết bị qua Internet</v>
       </c>
@@ -26693,7 +26693,7 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F92" s="240" t="s">
+      <c r="F92" s="216" t="s">
         <v>814</v>
       </c>
       <c r="G92" s="210" t="str">
@@ -26723,19 +26723,19 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="93" spans="1:14" ht="42">
-      <c r="A93" s="239" t="s">
+    <row r="93" spans="1:14" ht="41.4">
+      <c r="A93" s="215" t="s">
         <v>474</v>
       </c>
       <c r="B93" s="210">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="C93" s="240" t="str">
+      <c r="C93" s="216" t="str">
         <f>VLOOKUP(A93,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Xây dựng hệ thống cảm biến ứng dụng trong mô hình nhà thông minh</v>
       </c>
-      <c r="D93" s="240" t="str">
+      <c r="D93" s="216" t="str">
         <f>VLOOKUP(A93,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Xây dựng hệ thống cảm biến ứng dụng trong mô hình nhà thông minh</v>
       </c>
@@ -26770,19 +26770,19 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="94" spans="1:14" ht="42">
-      <c r="A94" s="239" t="s">
+    <row r="94" spans="1:14" ht="41.4">
+      <c r="A94" s="215" t="s">
         <v>479</v>
       </c>
       <c r="B94" s="210">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="C94" s="240" t="str">
+      <c r="C94" s="216" t="str">
         <f>VLOOKUP(A94,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Nghiên cứu, xây dựng xe robot điều khiển bằng cử chỉ cơ thể</v>
       </c>
-      <c r="D94" s="240" t="str">
+      <c r="D94" s="216" t="str">
         <f>VLOOKUP(A94,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Nghiên cứu, xây dựng xe robot điều khiển bằng cử chỉ cơ thể</v>
       </c>
@@ -26790,7 +26790,7 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F94" s="240" t="s">
+      <c r="F94" s="216" t="s">
         <v>814</v>
       </c>
       <c r="G94" s="210" t="str">
@@ -26820,19 +26820,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:14" ht="42">
-      <c r="A95" s="239" t="s">
+    <row r="95" spans="1:14" ht="41.4">
+      <c r="A95" s="215" t="s">
         <v>483</v>
       </c>
       <c r="B95" s="210">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="C95" s="240" t="str">
+      <c r="C95" s="216" t="str">
         <f>VLOOKUP(A95,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Phân loại trái cây bằng khối lượng và lưu dữ liệu trên My SQL</v>
       </c>
-      <c r="D95" s="240" t="str">
+      <c r="D95" s="216" t="str">
         <f>VLOOKUP(A95,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Phân loại trái cây bằng khối lượng và lưu dữ liệu trên My SQL</v>
       </c>
@@ -26867,19 +26867,19 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="96" spans="1:14" ht="56">
-      <c r="A96" s="239" t="s">
+    <row r="96" spans="1:14" ht="41.4">
+      <c r="A96" s="215" t="s">
         <v>487</v>
       </c>
       <c r="B96" s="210">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="C96" s="240" t="str">
+      <c r="C96" s="216" t="str">
         <f>VLOOKUP(A96,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Nghiên cứu, xây dựng xe robot thám hiểm sử dụng raspberry Pi 4</v>
       </c>
-      <c r="D96" s="240" t="str">
+      <c r="D96" s="216" t="str">
         <f>VLOOKUP(A96,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Nghiên cứu, xây dựng xe robot thám hiểm sử dụng raspberry Pi 4</v>
       </c>
@@ -26887,7 +26887,7 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="F96" s="240" t="s">
+      <c r="F96" s="216" t="s">
         <v>814</v>
       </c>
       <c r="G96" s="210" t="str">
@@ -26917,20 +26917,20 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="97" spans="1:14" ht="42">
-      <c r="A97" s="239" t="s">
+    <row r="97" spans="1:14" ht="41.4">
+      <c r="A97" s="215" t="s">
         <v>490</v>
       </c>
       <c r="B97" s="210">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="C97" s="240" t="str">
+      <c r="C97" s="216" t="str">
         <f>VLOOKUP(A97,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v xml:space="preserve">Dự kiến nhà thông minh mở khóa bằng sinh trắc học 
 </v>
       </c>
-      <c r="D97" s="240" t="str">
+      <c r="D97" s="216" t="str">
         <f>VLOOKUP(A97,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v xml:space="preserve">Dự kiến nhà thông minh mở khóa bằng sinh trắc học 
 </v>
@@ -26966,19 +26966,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:14" ht="28">
-      <c r="A98" s="239" t="s">
+    <row r="98" spans="1:14" ht="27.6">
+      <c r="A98" s="215" t="s">
         <v>494</v>
       </c>
       <c r="B98" s="210">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="C98" s="240" t="str">
+      <c r="C98" s="216" t="str">
         <f>VLOOKUP(A98,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Hệ thống chấm thi trắc nghiệm tự động</v>
       </c>
-      <c r="D98" s="240" t="str">
+      <c r="D98" s="216" t="str">
         <f>VLOOKUP(A98,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Hệ thống chấm thi trắc nghiệm tự động</v>
       </c>
@@ -27013,19 +27013,19 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="99" spans="1:14" ht="56">
-      <c r="A99" s="239" t="s">
+    <row r="99" spans="1:14" ht="55.2">
+      <c r="A99" s="215" t="s">
         <v>499</v>
       </c>
       <c r="B99" s="210">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="C99" s="240" t="str">
+      <c r="C99" s="216" t="str">
         <f>VLOOKUP(A99,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Thiết kế và triển khai IoT cho vườn thông minh sử dụng pin năng lượng Mặt trời</v>
       </c>
-      <c r="D99" s="240" t="str">
+      <c r="D99" s="216" t="str">
         <f>VLOOKUP(A99,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Thiết kế và triển khai IoT cho vườn thông minh sử dụng pin năng lượng Mặt trời</v>
       </c>
@@ -27060,19 +27060,19 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="100" spans="1:14" ht="28">
-      <c r="A100" s="239" t="s">
+    <row r="100" spans="1:14" ht="27.6">
+      <c r="A100" s="215" t="s">
         <v>501</v>
       </c>
       <c r="B100" s="210">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="C100" s="240" t="str">
+      <c r="C100" s="216" t="str">
         <f>VLOOKUP(A100,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Thiết kế hệ thống nhà thông minh</v>
       </c>
-      <c r="D100" s="240" t="str">
+      <c r="D100" s="216" t="str">
         <f>VLOOKUP(A100,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Thiết kế hệ thống nhà thông minh</v>
       </c>
@@ -27107,19 +27107,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:14" ht="28">
-      <c r="A101" s="239" t="s">
+    <row r="101" spans="1:14" ht="27.6">
+      <c r="A101" s="215" t="s">
         <v>505</v>
       </c>
       <c r="B101" s="210">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="C101" s="240" t="str">
+      <c r="C101" s="216" t="str">
         <f>VLOOKUP(A101,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Xây dựng Robot tự hành ứng dụng SLAM</v>
       </c>
-      <c r="D101" s="240" t="str">
+      <c r="D101" s="216" t="str">
         <f>VLOOKUP(A101,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Xây dựng Robot tự hành ứng dụng SLAM</v>
       </c>
@@ -27154,19 +27154,19 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="102" spans="1:14" ht="42">
-      <c r="A102" s="239" t="s">
+    <row r="102" spans="1:14" ht="41.4">
+      <c r="A102" s="215" t="s">
         <v>508</v>
       </c>
       <c r="B102" s="210">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="C102" s="240" t="str">
+      <c r="C102" s="216" t="str">
         <f>VLOOKUP(A102,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Ứng dụng thị giác máy tính điều khiển cánh tay Robot</v>
       </c>
-      <c r="D102" s="240" t="str">
+      <c r="D102" s="216" t="str">
         <f>VLOOKUP(A102,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Ứng dụng thị giác máy tính điều khiển cánh tay Robot</v>
       </c>
@@ -27201,19 +27201,19 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="103" spans="1:14" ht="84">
-      <c r="A103" s="239" t="s">
+    <row r="103" spans="1:14" ht="82.8">
+      <c r="A103" s="215" t="s">
         <v>510</v>
       </c>
       <c r="B103" s="210">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="C103" s="240" t="str">
+      <c r="C103" s="216" t="str">
         <f>VLOOKUP(A103,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Chuyển Đổi Ngôn Ngữ Thường Sang Ngôn Ngữ Ký Hiệu Bằng AI Giúp  Người Khiếm Thị Đọc Các Thông Tin trên mạng xã hội</v>
       </c>
-      <c r="D103" s="240" t="str">
+      <c r="D103" s="216" t="str">
         <f>VLOOKUP(A103,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Chuyển Đổi Ngôn Ngữ Thường Sang Ngôn Ngữ Ký Hiệu Bằng AI Giúp  Người Khiếm Thị Đọc Các Thông Tin trên mạng xã hội</v>
       </c>
@@ -27248,19 +27248,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:14" ht="42">
-      <c r="A104" s="239" t="s">
+    <row r="104" spans="1:14" ht="41.4">
+      <c r="A104" s="215" t="s">
         <v>514</v>
       </c>
       <c r="B104" s="210">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="C104" s="240" t="str">
+      <c r="C104" s="216" t="str">
         <f>VLOOKUP(A104,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Mô hình khoá cửa thông minh nhận diện khuôn mặt bằng xử lý ảnh</v>
       </c>
-      <c r="D104" s="240" t="str">
+      <c r="D104" s="216" t="str">
         <f>VLOOKUP(A104,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Mô hình khoá cửa thông minh nhận diện khuôn mặt bằng xử lý ảnh</v>
       </c>
@@ -27295,19 +27295,19 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="105" spans="1:14" ht="28">
-      <c r="A105" s="239" t="s">
+    <row r="105" spans="1:14" ht="27.6">
+      <c r="A105" s="215" t="s">
         <v>519</v>
       </c>
       <c r="B105" s="210">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="C105" s="240" t="str">
+      <c r="C105" s="216" t="str">
         <f>VLOOKUP(A105,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Hệ thống báo cháy và chữa cháy tự động</v>
       </c>
-      <c r="D105" s="240" t="str">
+      <c r="D105" s="216" t="str">
         <f>VLOOKUP(A105,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Hệ thống báo cháy và chữa cháy tự động</v>
       </c>
@@ -27342,19 +27342,19 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="106" spans="1:14" ht="28">
-      <c r="A106" s="239" t="s">
+    <row r="106" spans="1:14" ht="27.6">
+      <c r="A106" s="215" t="s">
         <v>522</v>
       </c>
       <c r="B106" s="210">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="C106" s="240" t="str">
+      <c r="C106" s="216" t="str">
         <f>VLOOKUP(A106,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Tìm hiểu, xây dựng hệ thống khóa dựa trên RFID</v>
       </c>
-      <c r="D106" s="240" t="str">
+      <c r="D106" s="216" t="str">
         <f>VLOOKUP(A106,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Tìm hiểu, xây dựng hệ thống khóa dựa trên RFID</v>
       </c>
@@ -27389,19 +27389,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:14" ht="28">
-      <c r="A107" s="239" t="s">
+    <row r="107" spans="1:14" ht="27.6">
+      <c r="A107" s="215" t="s">
         <v>526</v>
       </c>
       <c r="B107" s="210">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="C107" s="240" t="str">
+      <c r="C107" s="216" t="str">
         <f>VLOOKUP(A107,'DS SV các Hội đồng phân PB'!$B$5:$J$136,9,FALSE)</f>
         <v>Thiết kế hệ thống khóa cửa thông minh đa năng</v>
       </c>
-      <c r="D107" s="240" t="str">
+      <c r="D107" s="216" t="str">
         <f>VLOOKUP(A107,'Danh sách các đồ án '!$B$14:$J$202,9,FALSE)</f>
         <v>Thiết kế hệ thống khóa cửa thông minh đa năng</v>
       </c>

</xml_diff>